<commit_message>
Second Payment Page Added
</commit_message>
<xml_diff>
--- a/result/Summary.xlsx
+++ b/result/Summary.xlsx
@@ -618,10 +618,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Payment with Paypal execution success
</commit_message>
<xml_diff>
--- a/result/Summary.xlsx
+++ b/result/Summary.xlsx
@@ -618,10 +618,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>